<commit_message>
30-8-2025 (Sunil Final Push)
(Sunil Final Push)
</commit_message>
<xml_diff>
--- a/public/admin/approvedcandidates_formate.xlsx
+++ b/public/admin/approvedcandidates_formate.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="217">
   <si>
     <t>Client_Name</t>
   </si>
@@ -646,6 +646,9 @@
     <t>7th</t>
   </si>
   <si>
+    <t>Unique Punch Systems Pvt Ltd</t>
+  </si>
+  <si>
     <t>JHARKHAND</t>
   </si>
   <si>
@@ -750,7 +753,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,6 +772,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.1"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1258,137 +1267,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1397,28 +1406,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
@@ -1959,30 +1971,30 @@
   <sheetPr/>
   <dimension ref="A1:CB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="BW1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="BX1" workbookViewId="0">
       <selection activeCell="BY6" sqref="BY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="6" width="34.2222222222222" customWidth="1"/>
-    <col min="7" max="9" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="7" max="9" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="10" max="15" width="34.2222222222222" customWidth="1"/>
-    <col min="16" max="16" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="16" max="16" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="17" max="18" width="34.2222222222222" customWidth="1"/>
-    <col min="19" max="19" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="19" max="19" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="20" max="21" width="34.2222222222222" customWidth="1"/>
-    <col min="22" max="22" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="22" max="22" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="23" max="26" width="34.2222222222222" customWidth="1"/>
-    <col min="27" max="27" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="27" max="27" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="28" max="30" width="34.2222222222222" customWidth="1"/>
-    <col min="31" max="31" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="31" max="31" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="32" max="33" width="34.2222222222222" customWidth="1"/>
-    <col min="34" max="34" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="34" max="34" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="35" max="36" width="34.2222222222222" customWidth="1"/>
-    <col min="37" max="37" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="37" max="37" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="38" max="39" width="34.2222222222222" customWidth="1"/>
-    <col min="40" max="40" width="34.2222222222222" style="6" customWidth="1"/>
+    <col min="40" max="40" width="34.2222222222222" style="7" customWidth="1"/>
     <col min="41" max="72" width="34.2222222222222" customWidth="1"/>
     <col min="73" max="73" width="77.8888888888889" customWidth="1"/>
     <col min="74" max="77" width="34.2222222222222" customWidth="1"/>
@@ -1991,245 +2003,245 @@
     <col min="80" max="80" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="19.4" customHeight="1" spans="1:80">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="6" customFormat="1" ht="19.4" customHeight="1" spans="1:80">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AK1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AN1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="7" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="7" t="s">
+      <c r="AR1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="7" t="s">
+      <c r="AS1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="7" t="s">
+      <c r="AT1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="7" t="s">
+      <c r="AU1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="7" t="s">
+      <c r="AV1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="7" t="s">
+      <c r="AX1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="7" t="s">
+      <c r="AY1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="7" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BA1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BD1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BF1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BG1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="11" t="s">
+      <c r="BH1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="11" t="s">
+      <c r="BI1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="11" t="s">
+      <c r="BJ1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="11" t="s">
+      <c r="BK1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="11" t="s">
+      <c r="BL1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="11" t="s">
+      <c r="BM1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BN1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="11" t="s">
+      <c r="BO1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="11" t="s">
+      <c r="BP1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="11" t="s">
+      <c r="BQ1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="11" t="s">
+      <c r="BR1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="11" t="s">
+      <c r="BS1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="11" t="s">
+      <c r="BT1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="11" t="s">
+      <c r="BU1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="11" t="s">
+      <c r="BV1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="11" t="s">
+      <c r="BW1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="11" t="s">
+      <c r="BX1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="11" t="s">
+      <c r="BY1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="11" t="s">
+      <c r="BZ1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CA1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CB1" s="8" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2252,13 +2264,13 @@
       <c r="F2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>88</v>
       </c>
       <c r="J2" t="s">
@@ -2279,7 +2291,7 @@
       <c r="O2" t="s">
         <v>94</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>95</v>
       </c>
       <c r="Q2" t="s">
@@ -2288,19 +2300,19 @@
       <c r="R2" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="13" t="s">
         <v>99</v>
       </c>
       <c r="U2" t="s">
         <v>100</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="W2" s="13" t="s">
         <v>101</v>
       </c>
       <c r="X2" t="s">
@@ -2312,7 +2324,7 @@
       <c r="Z2" t="s">
         <v>104</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="7" t="s">
         <v>104</v>
       </c>
       <c r="AB2" t="s">
@@ -2324,7 +2336,7 @@
       <c r="AD2" t="s">
         <v>104</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="7" t="s">
         <v>98</v>
       </c>
       <c r="AF2" t="s">
@@ -2333,7 +2345,7 @@
       <c r="AG2" t="s">
         <v>104</v>
       </c>
-      <c r="AH2" s="6">
+      <c r="AH2" s="7">
         <v>45877</v>
       </c>
       <c r="AI2" t="s">
@@ -2342,7 +2354,7 @@
       <c r="AJ2" t="s">
         <v>104</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AK2" s="7" t="s">
         <v>98</v>
       </c>
       <c r="AL2" t="s">
@@ -2351,7 +2363,7 @@
       <c r="AM2" t="s">
         <v>104</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AN2" s="7" t="s">
         <v>104</v>
       </c>
       <c r="AO2" t="s">
@@ -2378,7 +2390,7 @@
       <c r="AV2">
         <v>1587423690</v>
       </c>
-      <c r="AW2" s="10" t="s">
+      <c r="AW2" s="11" t="s">
         <v>110</v>
       </c>
       <c r="AX2" t="s">
@@ -2405,7 +2417,7 @@
       <c r="BE2" t="s">
         <v>114</v>
       </c>
-      <c r="BF2" s="12" t="s">
+      <c r="BF2" s="13" t="s">
         <v>115</v>
       </c>
       <c r="BG2" t="s">
@@ -2459,36 +2471,36 @@
       <c r="CA2" t="s">
         <v>117</v>
       </c>
-      <c r="CB2" s="10" t="s">
+      <c r="CB2" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="3" spans="80:80">
-      <c r="CB3" s="10"/>
+      <c r="CB3" s="11"/>
     </row>
     <row r="4" spans="80:80">
-      <c r="CB4" s="10"/>
+      <c r="CB4" s="11"/>
     </row>
     <row r="5" spans="80:80">
-      <c r="CB5" s="10"/>
+      <c r="CB5" s="11"/>
     </row>
     <row r="6" spans="80:80">
-      <c r="CB6" s="10"/>
+      <c r="CB6" s="11"/>
     </row>
     <row r="7" spans="80:80">
-      <c r="CB7" s="10"/>
+      <c r="CB7" s="11"/>
     </row>
     <row r="8" spans="80:80">
-      <c r="CB8" s="10"/>
+      <c r="CB8" s="11"/>
     </row>
     <row r="9" spans="80:80">
-      <c r="CB9" s="10"/>
+      <c r="CB9" s="11"/>
     </row>
     <row r="10" spans="80:80">
-      <c r="CB10" s="10"/>
+      <c r="CB10" s="11"/>
     </row>
     <row r="11" spans="80:80">
-      <c r="CB11" s="10"/>
+      <c r="CB11" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="10">
@@ -2500,6 +2512,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
       <formula1>list!$AB$14:$AB$27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CA2 CA3:CA4 CA5:CA11">
+      <formula1>list!$Z$15:$Z$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A11">
       <formula1>list!$B$2:$B$75</formula1>
@@ -2519,9 +2534,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU11">
       <formula1>list!$AC$2:$AC$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CA2:CA11 BY2:BZ11">
-      <formula1>list!$Z$15:$Z$17</formula1>
-    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="CB2" r:id="rId1" display="ffemp@123"/>
@@ -2537,8 +2549,8 @@
   <sheetPr/>
   <dimension ref="A1:CH38"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA30" sqref="AA30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3007,119 +3019,125 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" s="1" customFormat="1" spans="15:28">
+    <row r="18" s="1" customFormat="1" ht="15" spans="1:28">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="O18" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P18" s="1">
         <v>33</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" spans="15:28">
       <c r="O19" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="P19" s="1">
         <v>9</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" spans="15:28">
       <c r="O20" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P20" s="1">
         <v>10</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="15:28">
       <c r="O21" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="P21" s="1">
         <v>27</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="15:28">
       <c r="O22" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="P22" s="1">
         <v>11</v>
       </c>
-      <c r="AB22" s="4" t="s">
-        <v>194</v>
+      <c r="AB22" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="15:28">
       <c r="O23" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P23" s="1">
         <v>12</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" spans="15:28">
       <c r="O24" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="P24" s="1">
         <v>13</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="15:28">
       <c r="O25" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="P25" s="1">
         <v>14</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="15:28">
       <c r="O26" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="P26" s="1">
         <v>15</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="15:28">
       <c r="O27" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="P27" s="1">
         <v>16</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="15:16">
       <c r="O28" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="P28" s="1">
         <v>17</v>
@@ -3127,7 +3145,7 @@
     </row>
     <row r="29" s="1" customFormat="1" spans="15:16">
       <c r="O29" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="P29" s="1">
         <v>26</v>
@@ -3135,7 +3153,7 @@
     </row>
     <row r="30" s="1" customFormat="1" spans="15:16">
       <c r="O30" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="P30" s="1">
         <v>18</v>
@@ -3143,7 +3161,7 @@
     </row>
     <row r="31" s="1" customFormat="1" spans="15:16">
       <c r="O31" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P31" s="1">
         <v>19</v>
@@ -3151,7 +3169,7 @@
     </row>
     <row r="32" s="1" customFormat="1" spans="15:16">
       <c r="O32" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P32" s="1">
         <v>20</v>
@@ -3159,7 +3177,7 @@
     </row>
     <row r="33" s="1" customFormat="1" spans="15:16">
       <c r="O33" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="P33" s="1">
         <v>21</v>
@@ -3167,7 +3185,7 @@
     </row>
     <row r="34" s="1" customFormat="1" spans="15:16">
       <c r="O34" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P34" s="1">
         <v>36</v>
@@ -3175,7 +3193,7 @@
     </row>
     <row r="35" s="1" customFormat="1" spans="15:16">
       <c r="O35" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="P35" s="1">
         <v>22</v>
@@ -3183,7 +3201,7 @@
     </row>
     <row r="36" s="1" customFormat="1" spans="15:16">
       <c r="O36" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P36" s="1">
         <v>23</v>
@@ -3191,7 +3209,7 @@
     </row>
     <row r="37" s="1" customFormat="1" spans="15:16">
       <c r="O37" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="P37" s="1">
         <v>32</v>
@@ -3199,7 +3217,7 @@
     </row>
     <row r="38" s="1" customFormat="1" spans="15:16">
       <c r="O38" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="P38" s="1">
         <v>24</v>

</xml_diff>